<commit_message>
applied minor changes to Chi-squared test in Excel
</commit_message>
<xml_diff>
--- a/EA1/Aufgabe_1_2.xlsx
+++ b/EA1/Aufgabe_1_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="2756" documentId="11_0C4960CD9ED4E780DF6DC377A018FCC687AFA1B0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19370E8E-B70F-42A8-A050-92540FB8225F}"/>
+  <xr:revisionPtr revIDLastSave="3698" documentId="11_0C4960CD9ED4E780DF6DC377A018FCC687AFA1B0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FF5CEFC-14F0-404B-8B0F-F8E34F5B0C73}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,9 +14,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datensätze!$A$1:$D$1</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Datensätze!$C$2:$C$101</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Datensätze!$A$2:$A$101</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Datensätze!$C$2:$C$101</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Datensätze!$A$2:$A$101</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Aufgabe a)'!$B$2:$B$3</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'Aufgabe b)'!$B$2</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
@@ -51,7 +50,7 @@
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Aufgabe a)'!$E$16</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Aufgabe b)'!$E$17</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Aufgabe b)'!$E$18</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Datensätze!$D$16</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
@@ -103,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Datensatz 1</t>
   </si>
@@ -141,19 +140,10 @@
     <t>α</t>
   </si>
   <si>
-    <t>Prüfvariable</t>
-  </si>
-  <si>
     <t>W'lichkeit</t>
   </si>
   <si>
-    <t>Ablehnung ab</t>
-  </si>
-  <si>
     <t>Folgt N(μ;σ)</t>
-  </si>
-  <si>
-    <t>Parametrisierung erfolgte über Solver via Minimierung der quadratischen Abweichung</t>
   </si>
   <si>
     <t>Parameter für Exp(λ)</t>
@@ -162,13 +152,16 @@
     <t>λ</t>
   </si>
   <si>
-    <t>Folgt Exp(λ)</t>
-  </si>
-  <si>
     <t>Χ²-Anpassungstest</t>
   </si>
   <si>
-    <t>Prüfwert</t>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Χ²(Prüfwert)</t>
+  </si>
+  <si>
+    <t>Parametrisierung erfolgte über Solver via Minimierung der summierten quadratischen Abweichung</t>
   </si>
 </sst>
 </file>
@@ -178,7 +171,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -492,33 +485,36 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -527,14 +523,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -547,9 +535,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -560,6 +545,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1103,7 +1093,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Aufgabe b)'!$B$4</c:f>
+              <c:f>'Aufgabe b)'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1125,7 +1115,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Aufgabe b)'!$B$6:$B$15</c:f>
+              <c:f>'Aufgabe b)'!$B$7:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1173,7 +1163,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Aufgabe b)'!$D$4</c:f>
+              <c:f>'Aufgabe b)'!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1195,39 +1185,39 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Aufgabe b)'!$D$6:$D$15</c:f>
+              <c:f>'Aufgabe b)'!$D$7:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>18.779915008455113</c:v>
+                  <c:v>18.779915018714938</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.245702115635011</c:v>
+                  <c:v>15.245702122028737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.376596640295368</c:v>
+                  <c:v>12.37659664391475</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.047431284878543</c:v>
+                  <c:v>10.047431286541375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1565941234348127</c:v>
+                  <c:v>8.1565941237493167</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6215956902914597</c:v>
+                  <c:v>6.6215956897062389</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3754703031885898</c:v>
+                  <c:v>5.3754703020311272</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3638546253781607</c:v>
+                  <c:v>4.363854623884567</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5426160163397058</c:v>
+                  <c:v>3.5426160146775021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8759272057874763</c:v>
+                  <c:v>2.8759272040730144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1500,7 +1490,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3936,13 +3926,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -3977,15 +3967,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4415,7 +4405,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D4:D11" si="0">D4+0.1</f>
+        <f t="shared" ref="D5:D11" si="0">D4+0.1</f>
         <v>0.30100000000000005</v>
       </c>
       <c r="G5" s="3"/>
@@ -5336,10 +5326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47051651-8ECA-4BE6-BD58-C4242B9F4786}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5347,368 +5337,318 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="13">
         <v>25.93577875516009</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="15">
         <v>10.045590380599204</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>_xlfn.NORM.DIST(A6,$B$2,$B$3,TRUE)</f>
         <v>5.6330459348821957E-2</v>
       </c>
-      <c r="D6" s="10">
-        <f>C6*$B$16</f>
+      <c r="D6" s="7">
+        <f t="shared" ref="D6:D15" si="0">C6*$B$16</f>
         <v>5.6330459348821957</v>
       </c>
-      <c r="E6" s="8">
-        <f t="shared" ref="E6:E15" si="0">(B6-D6)^2</f>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6:E15" si="1">(B6-D6)^2</f>
         <v>2.6668390254352645</v>
       </c>
-      <c r="F6" s="8">
-        <f t="shared" ref="F6:F15" si="1">E6/D6</f>
-        <v>0.47342753037412189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>15</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f>_xlfn.NORM.DIST(A7,$B$2,$B$3,TRUE)-SUM($C$6:C6)</f>
         <v>8.183142577748255E-2</v>
       </c>
-      <c r="D7" s="10">
-        <f>C7*$B$16</f>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
         <v>8.1831425777482547</v>
       </c>
-      <c r="E7" s="8">
-        <f t="shared" si="0"/>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
         <v>3.3009708927912569</v>
       </c>
-      <c r="F7" s="8">
-        <f t="shared" si="1"/>
-        <v>0.40338670155489104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>20</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>15</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f>_xlfn.NORM.DIST(A8,$B$2,$B$3,TRUE)-SUM($C$6:C7)</f>
         <v>0.13913718416778748</v>
       </c>
-      <c r="D8" s="10">
-        <f>C8*$B$16</f>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
         <v>13.913718416778748</v>
       </c>
-      <c r="E8" s="8">
-        <f t="shared" si="0"/>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
         <v>1.1800076780456703</v>
       </c>
-      <c r="F8" s="8">
-        <f t="shared" si="1"/>
-        <v>8.4808937675688659E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>25</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>18</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f>_xlfn.NORM.DIST(A9,$B$2,$B$3,TRUE)-SUM($C$6:C8)</f>
         <v>0.18559186285353968</v>
       </c>
-      <c r="D9" s="10">
-        <f>C9*$B$16</f>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
         <v>18.559186285353967</v>
       </c>
-      <c r="E9" s="8">
-        <f t="shared" si="0"/>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
         <v>0.31268930172796783</v>
       </c>
-      <c r="F9" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6848222595552451E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>30</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f>_xlfn.NORM.DIST(A10,$B$2,$B$3,TRUE)-SUM($C$6:C9)</f>
         <v>0.19421506910806352</v>
       </c>
-      <c r="D10" s="10">
-        <f>C10*$B$16</f>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
         <v>19.42150691080635</v>
       </c>
-      <c r="E10" s="8">
-        <f t="shared" si="0"/>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
         <v>5.863695719082914</v>
       </c>
-      <c r="F10" s="8">
-        <f t="shared" si="1"/>
-        <v>0.3019176496454189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>35</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>19</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f>_xlfn.NORM.DIST(A11,$B$2,$B$3,TRUE)-SUM($C$6:C10)</f>
         <v>0.15944748391865693</v>
       </c>
-      <c r="D11" s="10">
-        <f>C11*$B$16</f>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
         <v>15.944748391865692</v>
       </c>
-      <c r="E11" s="8">
-        <f t="shared" si="0"/>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
         <v>9.3345623890072726</v>
       </c>
-      <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>0.58543177725961204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>40</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f>_xlfn.NORM.DIST(A12,$B$2,$B$3,TRUE)-SUM($C$6:C11)</f>
         <v>0.10269573853154024</v>
       </c>
-      <c r="D12" s="10">
-        <f>C12*$B$16</f>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
         <v>10.269573853154023</v>
       </c>
-      <c r="E12" s="8">
-        <f t="shared" si="0"/>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
         <v>1.6118177686123534</v>
       </c>
-      <c r="F12" s="8">
-        <f t="shared" si="1"/>
-        <v>0.15695079383623373</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>45</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>_xlfn.NORM.DIST(A13,$B$2,$B$3,TRUE)-SUM($C$6:C12)</f>
         <v>5.1887590703061259E-2</v>
       </c>
-      <c r="D13" s="10">
-        <f>C13*$B$16</f>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
         <v>5.1887590703061264</v>
       </c>
-      <c r="E13" s="8">
-        <f t="shared" si="0"/>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
         <v>3.5629986622833162E-2</v>
       </c>
-      <c r="F13" s="8">
-        <f t="shared" si="1"/>
-        <v>6.8667645076708221E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>50</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>_xlfn.NORM.DIST(A14,$B$2,$B$3,TRUE)-SUM($C$6:C13)</f>
         <v>2.0564349852737029E-2</v>
       </c>
-      <c r="D14" s="10">
-        <f>C14*$B$16</f>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
         <v>2.0564349852737029</v>
       </c>
-      <c r="E14" s="8">
-        <f t="shared" si="0"/>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
         <v>0.89031493701543718</v>
       </c>
-      <c r="F14" s="8">
-        <f t="shared" si="1"/>
-        <v>0.43294096015242611</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <f>2^64</f>
         <v>1.8446744073709552E+19</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f>_xlfn.NORM.DIST(A15,$B$2,$B$3,TRUE)-SUM($C$6:C14)</f>
         <v>8.2988357383093625E-3</v>
       </c>
-      <c r="D15" s="10">
-        <f>C15*$B$16</f>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
         <v>0.82988357383093625</v>
       </c>
-      <c r="E15" s="8">
-        <f t="shared" si="0"/>
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
         <v>0.68870674611440696</v>
       </c>
-      <c r="F15" s="8">
-        <f t="shared" si="1"/>
-        <v>0.82988357383093614</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f>SUM(B6:B15)</f>
         <v>100</v>
       </c>
-      <c r="C16" s="7">
-        <f t="shared" ref="C16:F16" si="2">SUM(C6:C15)</f>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:E16" si="2">SUM(C6:C15)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f t="shared" si="2"/>
         <v>25.885234444455378</v>
       </c>
-      <c r="F16" s="9">
-        <f t="shared" si="2"/>
-        <v>3.2924629114325521</v>
-      </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="19"/>
+      <c r="A18" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="22"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="16">
         <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="25">
-        <f>F16</f>
-        <v>3.2924629114325521</v>
+      <c r="A20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="32">
+        <f>1-B19</f>
+        <v>0.95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="25">
-        <f>_xlfn.CHISQ.INV.RT(B19,9)</f>
-        <v>16.918977604620451</v>
+      <c r="A21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="31">
+        <f>_xlfn.CHISQ.TEST(B6:B15,D6:D15)</f>
+        <v>0.95156296754536041</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="14" t="b">
-        <f>B20&lt;=B21</f>
+      <c r="A22" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="b">
+        <f>B21&gt;=B20</f>
         <v>1</v>
       </c>
     </row>
@@ -5716,7 +5656,7 @@
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C1:F3"/>
+    <mergeCell ref="C1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5725,10 +5665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14456AF-18E5-4ED0-8E08-2D996937DD51}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,412 +5676,362 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="28" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2.0849031340608808</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <f>_xlfn.EXPON.DIST(A6,$B$2,TRUE)</f>
+        <v>2.0827312331848633E-3</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" ref="D6:D17" si="0">C6*$B$18</f>
+        <v>0.20827312331848633</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6:E17" si="1">(B6-D6)^2</f>
+        <v>0.62683144725986473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <f>_xlfn.EXPON.DIST(A7,$B$2,TRUE)-SUM($C$6:C6)</f>
+        <v>0.18779915018714938</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>18.779915018714938</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>163.32622788557563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <f>_xlfn.EXPON.DIST(A8,$B$2,TRUE)-SUM($C$6:C7)</f>
+        <v>0.15245702122028737</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>15.245702122028737</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>52.500199241171742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.30100000000000005</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5">
+        <f>_xlfn.EXPON.DIST(A9,$B$2,TRUE)-SUM($C$6:C8)</f>
+        <v>0.1237659664391475</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>12.37659664391475</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.38863174437835285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="B10">
         <v>16</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="21">
-        <v>2.0849031327914775</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C10" s="5">
+        <f>_xlfn.EXPON.DIST(A10,$B$2,TRUE)-SUM($C$6:C9)</f>
+        <v>0.10047431286541375</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>10.047431286541375</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>35.43307428844647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.501</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5">
+        <f>_xlfn.EXPON.DIST(A11,$B$2,TRUE)-SUM($C$6:C10)</f>
+        <v>8.1565941237493167E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>8.1565941237493167</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>8.0849569770969154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5">
+        <f>_xlfn.EXPON.DIST(A12,$B$2,TRUE)-SUM($C$6:C11)</f>
+        <v>6.6215956897062389E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>6.6215956897062389</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>28.927232924986509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
+        <f>_xlfn.EXPON.DIST(A13,$B$2,TRUE)-SUM($C$6:C12)</f>
+        <v>5.3754703020311267E-2</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>5.3754703020311272</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
+        <v>1.8919185517696002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.80099999999999993</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5">
+        <f>_xlfn.EXPON.DIST(A14,$B$2,TRUE)-SUM($C$6:C13)</f>
+        <v>4.3638546238845666E-2</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>4.363854623884567</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>21.49384394847651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.90099999999999991</v>
+      </c>
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <f>_xlfn.EXPON.DIST(A5,$B$2,TRUE)</f>
-        <v>2.0827312319181036E-3</v>
-      </c>
-      <c r="D5" s="10">
-        <f>C5*$B$17</f>
-        <v>0.20827312319181035</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" ref="E5:E16" si="0">(B5-D5)^2</f>
-        <v>0.62683144746045028</v>
-      </c>
-      <c r="F5" s="8">
-        <f t="shared" ref="F5:F16" si="1">E5/D5</f>
-        <v>3.0096607658932841</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="B6" s="4">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6">
-        <f>_xlfn.EXPON.DIST(A6,$B$2,TRUE)-SUM($C$5:C5)</f>
-        <v>0.18779915008455114</v>
-      </c>
-      <c r="D6" s="10">
-        <f>C6*$B$17</f>
-        <v>18.779915008455113</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="C15" s="5">
+        <f>_xlfn.EXPON.DIST(A15,$B$2,TRUE)-SUM($C$6:C14)</f>
+        <v>3.5426160146775021E-2</v>
+      </c>
+      <c r="D15" s="7">
         <f t="shared" si="0"/>
-        <v>163.32622762333625</v>
-      </c>
-      <c r="F6" s="8">
+        <v>3.5426160146775021</v>
+      </c>
+      <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>8.6968565911934821</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="B7" s="4">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6">
-        <f>_xlfn.EXPON.DIST(A7,$B$2,TRUE)-SUM($C$5:C6)</f>
-        <v>0.1524570211563501</v>
-      </c>
-      <c r="D7" s="10">
-        <f>C7*$B$17</f>
-        <v>15.245702115635011</v>
-      </c>
-      <c r="E7" s="8">
+        <v>89.442111845834447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5">
+        <f>_xlfn.EXPON.DIST(A16,$B$2,TRUE)-SUM($C$6:C15)</f>
+        <v>2.8759272040730144E-2</v>
+      </c>
+      <c r="D16" s="7">
         <f t="shared" si="0"/>
-        <v>52.500199148517666</v>
-      </c>
-      <c r="F7" s="8">
+        <v>2.8759272040730144</v>
+      </c>
+      <c r="E16" s="7">
         <f t="shared" si="1"/>
-        <v>3.4436065161391842</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>0.30100000000000005</v>
-      </c>
-      <c r="B8" s="4">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6">
-        <f>_xlfn.EXPON.DIST(A8,$B$2,TRUE)-SUM($C$5:C7)</f>
-        <v>0.12376596640295368</v>
-      </c>
-      <c r="D8" s="10">
-        <f>C8*$B$17</f>
-        <v>12.376596640295368</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="0"/>
-        <v>0.38863174889102281</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="1"/>
-        <v>3.1400534426865516E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="B9" s="4">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6">
-        <f>_xlfn.EXPON.DIST(A9,$B$2,TRUE)-SUM($C$5:C8)</f>
-        <v>0.10047431284878544</v>
-      </c>
-      <c r="D9" s="10">
-        <f>C9*$B$17</f>
-        <v>10.047431284878543</v>
-      </c>
-      <c r="E9" s="8">
-        <f t="shared" si="0"/>
-        <v>35.433074308242709</v>
-      </c>
-      <c r="F9" s="8">
-        <f t="shared" si="1"/>
-        <v>3.5265804068319175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>0.501</v>
-      </c>
-      <c r="B10" s="4">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6">
-        <f>_xlfn.EXPON.DIST(A10,$B$2,TRUE)-SUM($C$5:C9)</f>
-        <v>8.1565941234348127E-2</v>
-      </c>
-      <c r="D10" s="10">
-        <f>C10*$B$17</f>
-        <v>8.1565941234348127</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" si="0"/>
-        <v>8.0849569788854403</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="1"/>
-        <v>0.99121727237309121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>0.60099999999999998</v>
-      </c>
-      <c r="B11" s="4">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6">
-        <f>_xlfn.EXPON.DIST(A11,$B$2,TRUE)-SUM($C$5:C10)</f>
-        <v>6.6215956902914597E-2</v>
-      </c>
-      <c r="D11" s="10">
-        <f>C11*$B$17</f>
-        <v>6.6215956902914597</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="0"/>
-        <v>28.927232918691399</v>
-      </c>
-      <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>4.3686196306283573</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>0.70099999999999996</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6">
-        <f>_xlfn.EXPON.DIST(A12,$B$2,TRUE)-SUM($C$5:C11)</f>
-        <v>5.3754703031885898E-2</v>
-      </c>
-      <c r="D12" s="10">
-        <f>C12*$B$17</f>
-        <v>5.3754703031885898</v>
-      </c>
-      <c r="E12" s="8">
-        <f t="shared" si="0"/>
-        <v>1.891918554953711</v>
-      </c>
-      <c r="F12" s="8">
-        <f t="shared" si="1"/>
-        <v>0.35195405206340252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>0.80099999999999993</v>
-      </c>
-      <c r="B13" s="4">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6">
-        <f>_xlfn.EXPON.DIST(A13,$B$2,TRUE)-SUM($C$5:C12)</f>
-        <v>4.3638546253781607E-2</v>
-      </c>
-      <c r="D13" s="10">
-        <f>C13*$B$17</f>
-        <v>4.3638546253781607</v>
-      </c>
-      <c r="E13" s="8">
-        <f t="shared" si="0"/>
-        <v>21.493843934627474</v>
-      </c>
-      <c r="F13" s="8">
-        <f t="shared" si="1"/>
-        <v>4.9254262068285266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>0.90099999999999991</v>
-      </c>
-      <c r="B14" s="4">
-        <v>13</v>
-      </c>
-      <c r="C14" s="6">
-        <f>_xlfn.EXPON.DIST(A14,$B$2,TRUE)-SUM($C$5:C13)</f>
-        <v>3.5426160163397058E-2</v>
-      </c>
-      <c r="D14" s="10">
-        <f>C14*$B$17</f>
-        <v>3.5426160163397058</v>
-      </c>
-      <c r="E14" s="8">
-        <f t="shared" si="0"/>
-        <v>89.442111814394266</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" si="1"/>
-        <v>25.247475707741945</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="B15" s="4">
-        <v>7</v>
-      </c>
-      <c r="C15" s="6">
-        <f>_xlfn.EXPON.DIST(A15,$B$2,TRUE)-SUM($C$5:C14)</f>
-        <v>2.8759272057874763E-2</v>
-      </c>
-      <c r="D15" s="10">
-        <f>C15*$B$17</f>
-        <v>2.8759272057874763</v>
-      </c>
-      <c r="E15" s="8">
-        <f t="shared" si="0"/>
-        <v>17.007976411963888</v>
-      </c>
-      <c r="F15" s="8">
-        <f t="shared" si="1"/>
-        <v>5.9139106086333726</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+        <v>17.007976426105024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <f>2^64</f>
         <v>1.8446744073709552E+19</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17">
         <v>0</v>
       </c>
-      <c r="C16" s="6">
-        <f>_xlfn.EXPON.DIST(A16,$B$2,TRUE)-SUM($C$5:C15)</f>
-        <v>0.12406023863123949</v>
-      </c>
-      <c r="D16" s="10">
-        <f>C16*$B$17</f>
-        <v>12.406023863123949</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="C17" s="5">
+        <f>_xlfn.EXPON.DIST(A17,$B$2,TRUE)-SUM($C$6:C16)</f>
+        <v>0.12406023847359948</v>
+      </c>
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
-        <v>153.90942809240087</v>
-      </c>
-      <c r="F16" s="8">
+        <v>12.406023847359949</v>
+      </c>
+      <c r="E17" s="7">
         <f t="shared" si="1"/>
-        <v>12.40602386312395</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+        <v>153.90942770126375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="5">
-        <f>SUM(B5:B16)</f>
+      <c r="B18" s="4">
+        <f>SUM(B6:B17)</f>
         <v>100</v>
       </c>
-      <c r="C17" s="7">
-        <f t="shared" ref="C17:F17" si="2">SUM(C5:C16)</f>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:E18" si="2">SUM(C6:C17)</f>
         <v>1</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D18" s="8">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="8">
         <f t="shared" si="2"/>
-        <v>573.03243298236509</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" si="2"/>
-        <v>72.912732155877379</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+        <v>573.03243298236487</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B21" s="16">
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="25">
-        <f>F17</f>
-        <v>72.912732155877379</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="25">
-        <f>_xlfn.CHISQ.INV.RT(B20,11)</f>
-        <v>19.675137572682498</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="14" t="b">
-        <f>B21&lt;=B22</f>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="32">
+        <f>1-B21</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="31">
+        <f>_xlfn.CHISQ.TEST(B6:B17,D6:D17)</f>
+        <v>3.4021516525979354E-11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="10" t="b">
+        <f>B23&gt;=B22</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F2"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C1:E3"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>